<commit_message>
avant le chat gbt
</commit_message>
<xml_diff>
--- a/server/anes/uploads/tp0_3.xlsx
+++ b/server/anes/uploads/tp0_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA6B968-8A51-4D4D-99C4-9CECE46B5562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE019C8C-6635-4764-857D-865ABB2C0EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
   <si>
     <t>Sexe</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>anes</t>
-  </si>
-  <si>
-    <t>Sur une échelle de 1 à 5</t>
   </si>
   <si>
     <t>Masculin</t>
@@ -198,13 +195,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:D14" totalsRowShown="0">
-  <autoFilter ref="A1:D14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:C14" totalsRowShown="0">
+  <autoFilter ref="A1:C14" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="3">
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sexe"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Spécialité"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="anes"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Sur une échelle de 1 à 5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -498,20 +494,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="37.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.5546875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,189 +517,147 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
-        <v>4</v>
-      </c>
-      <c r="D2" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6">
-        <v>4</v>
-      </c>
-      <c r="D3" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
         <v>1</v>
       </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="C6" s="4">
         <v>3</v>
       </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="6">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="4">
         <v>5</v>
       </c>
-      <c r="D8" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6">
         <v>4</v>
       </c>
-      <c r="D9" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6">
         <v>3</v>
       </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
-      <c r="D12" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="6">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="8">
-        <v>4</v>
-      </c>
-      <c r="D14" s="8">
         <v>4</v>
       </c>
     </row>

</xml_diff>